<commit_message>
Major updates and changes
Added:
- Excel sheet with all information about planets that is used by program
to store variables
- Mercury and Earth fully functional orbits with correct average orbit
speeds and distances, and initial position can be adjusted with data
from www.theplanetstoday.com
- All numbers replaced with variables from excel file
- distance between sun and planet can be calculated
- notes file added to keep track of websites and important notes

Need to add:
- Add more planets, should be easy since layout is ready
- Add calculations between planets such as max/min distances
</commit_message>
<xml_diff>
--- a/planets info.xlsx
+++ b/planets info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Earth</t>
   </si>
@@ -67,15 +67,21 @@
   <si>
     <t>Perihelion (km)</t>
   </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Orbit Days</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +100,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -118,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -126,14 +138,15 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,14 +464,14 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="6" width="17" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -478,6 +491,12 @@
       </c>
       <c r="F1" t="s">
         <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
@@ -500,8 +519,13 @@
       <c r="F2" s="5">
         <v>46001200</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="2">
+        <f>B2-F2</f>
+        <v>11907850</v>
+      </c>
+      <c r="H2" s="1">
+        <v>88</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="1"/>
       <c r="K2" s="2"/>
@@ -16879,20 +16903,33 @@
       <c r="XFC2" s="2"/>
       <c r="XFD2" s="1"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="7">
+        <v>108210000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>108207348.82252268</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="4">
-        <v>2500000</v>
+      <c r="E3" s="3">
+        <v>108900000</v>
       </c>
+      <c r="F3" s="3">
+        <v>107500000</v>
+      </c>
+      <c r="G3" s="2">
+        <f>B3-F3</f>
+        <v>710000</v>
+      </c>
+      <c r="H3">
+        <v>225</v>
+      </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -16913,88 +16950,177 @@
       <c r="F4" s="3">
         <v>147100000</v>
       </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G3:G10" si="0">B4-F4</f>
+        <v>2500000</v>
+      </c>
       <c r="H4" s="3">
-        <f>E4-(E4+F4)/2</f>
-        <v>2500000</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="3">
+        <v>227920000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>9.2999999999999999E-2</v>
+      </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>226932219.49332446</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3">
+        <v>249200000</v>
+      </c>
+      <c r="F5" s="3">
+        <v>206600000</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>21320000</v>
+      </c>
       <c r="H5" s="3">
-        <f>F4+I3</f>
-        <v>149600000</v>
+        <v>687</v>
       </c>
     </row>
     <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="3">
+        <v>778570000</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.8000000000000001E-2</v>
+      </c>
       <c r="D6" s="3">
         <f t="array" ref="D6:D9">B6:B9*SQRT(1-C6:C9^2)</f>
-        <v>0</v>
+        <v>777672570.14231288</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="3">
+        <v>816600000</v>
+      </c>
+      <c r="F6" s="3">
+        <v>740500000</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>38070000</v>
+      </c>
+      <c r="H6">
+        <v>4329</v>
+      </c>
     </row>
     <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3">
+        <v>1433000000</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5.6000000000000001E-2</v>
+      </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>1430751291.628283</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3">
+        <v>1514500000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1352600000</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>80400000</v>
+      </c>
+      <c r="H7">
+        <v>10753</v>
+      </c>
     </row>
     <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3">
+        <v>1870000000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4.5999999999999999E-2</v>
+      </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>1868020492.2858851</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3">
+        <v>3003600000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2741300000</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>-871300000</v>
+      </c>
+      <c r="H8">
+        <v>30660</v>
+      </c>
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3">
+        <v>4495000000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.01</v>
+      </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>4494775244.380969</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="3">
+        <v>4545700000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4444500000</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>50500000</v>
+      </c>
+      <c r="H9">
+        <v>60225</v>
+      </c>
     </row>
     <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3">
+        <v>5906000000</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.24879999999999999</v>
+      </c>
       <c r="D10" s="3">
         <f t="array" ref="D10">B10:B13*SQRT(1-C10:C13^2)</f>
-        <v>0</v>
+        <v>5720285134.7809725</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="3">
+        <v>7375900000</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4436800000</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>1469200000</v>
+      </c>
+      <c r="H10">
+        <v>90520</v>
+      </c>
     </row>
     <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>

</xml_diff>